<commit_message>
Actualiza datos y proyeccion inicial GAMLSS
</commit_message>
<xml_diff>
--- a/Data/Poblacion_Distrital.xlsx
+++ b/Data/Poblacion_Distrital.xlsx
@@ -1400,20 +1400,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA477"/>
+  <dimension ref="A1:AB477"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1498,6 +1498,9 @@
       <c r="AA1" s="0" t="n">
         <v>2021</v>
       </c>
+      <c r="AB1" s="0" t="n">
+        <v>2022</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -1581,6 +1584,9 @@
       <c r="AA2" s="2" t="n">
         <v>2973</v>
       </c>
+      <c r="AB2" s="2" t="n">
+        <v>2946</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1664,6 +1670,9 @@
       <c r="AA3" s="2" t="n">
         <v>15309</v>
       </c>
+      <c r="AB3" s="2" t="n">
+        <v>15408</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -1747,6 +1756,9 @@
       <c r="AA4" s="2" t="n">
         <v>23859</v>
       </c>
+      <c r="AB4" s="2" t="n">
+        <v>24030</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1830,6 +1842,9 @@
       <c r="AA5" s="2" t="n">
         <v>15639</v>
       </c>
+      <c r="AB5" s="2" t="n">
+        <v>15682</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1913,6 +1928,9 @@
       <c r="AA6" s="2" t="n">
         <v>21929</v>
       </c>
+      <c r="AB6" s="2" t="n">
+        <v>21990</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1996,6 +2014,9 @@
       <c r="AA7" s="2" t="n">
         <v>23696</v>
       </c>
+      <c r="AB7" s="2" t="n">
+        <v>23745</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -2079,6 +2100,9 @@
       <c r="AA8" s="2" t="n">
         <v>42301</v>
       </c>
+      <c r="AB8" s="2" t="n">
+        <v>42861</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -2162,6 +2186,9 @@
       <c r="AA9" s="2" t="n">
         <v>10097</v>
       </c>
+      <c r="AB9" s="2" t="n">
+        <v>10119</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -2245,6 +2272,9 @@
       <c r="AA10" s="2" t="n">
         <v>88616</v>
       </c>
+      <c r="AB10" s="2" t="n">
+        <v>89531</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -2328,6 +2358,9 @@
       <c r="AA11" s="2" t="n">
         <v>60316</v>
       </c>
+      <c r="AB11" s="2" t="n">
+        <v>60723</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -2411,6 +2444,9 @@
       <c r="AA12" s="2" t="n">
         <v>44943</v>
       </c>
+      <c r="AB12" s="2" t="n">
+        <v>44923</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -2494,6 +2530,9 @@
       <c r="AA13" s="2" t="n">
         <v>70642</v>
       </c>
+      <c r="AB13" s="2" t="n">
+        <v>13752</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -2577,6 +2616,9 @@
       <c r="AA14" s="2" t="n">
         <v>28032</v>
       </c>
+      <c r="AB14" s="2" t="n">
+        <v>28329</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -2660,6 +2702,9 @@
       <c r="AA15" s="2" t="n">
         <v>28872</v>
       </c>
+      <c r="AB15" s="2" t="n">
+        <v>29121</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -2743,6 +2788,9 @@
       <c r="AA16" s="2" t="n">
         <v>37411</v>
       </c>
+      <c r="AB16" s="2" t="n">
+        <v>37479</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -2826,6 +2874,9 @@
       <c r="AA17" s="2" t="n">
         <v>38327</v>
       </c>
+      <c r="AB17" s="2" t="n">
+        <v>38716</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -2909,6 +2960,9 @@
       <c r="AA18" s="2" t="n">
         <v>24216</v>
       </c>
+      <c r="AB18" s="2" t="n">
+        <v>24505</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -2992,6 +3046,9 @@
       <c r="AA19" s="2" t="n">
         <v>18243</v>
       </c>
+      <c r="AB19" s="2" t="n">
+        <v>18412</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -3075,6 +3132,9 @@
       <c r="AA20" s="2" t="n">
         <v>11277</v>
       </c>
+      <c r="AB20" s="2" t="n">
+        <v>11343</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -3158,6 +3218,9 @@
       <c r="AA21" s="2" t="n">
         <v>4555</v>
       </c>
+      <c r="AB21" s="2" t="n">
+        <v>4586</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -3241,6 +3304,9 @@
       <c r="AA22" s="2" t="n">
         <v>14748</v>
       </c>
+      <c r="AB22" s="2" t="n">
+        <v>14919</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -3324,6 +3390,9 @@
       <c r="AA23" s="2" t="n">
         <v>4734</v>
       </c>
+      <c r="AB23" s="2" t="n">
+        <v>4769</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -3407,6 +3476,9 @@
       <c r="AA24" s="2" t="n">
         <v>3753</v>
       </c>
+      <c r="AB24" s="2" t="n">
+        <v>3787</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -3490,6 +3562,9 @@
       <c r="AA25" s="2" t="n">
         <v>15572</v>
       </c>
+      <c r="AB25" s="2" t="n">
+        <v>15713</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -3573,6 +3648,9 @@
       <c r="AA26" s="2" t="n">
         <v>26666</v>
       </c>
+      <c r="AB26" s="2" t="n">
+        <v>26781</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -3656,6 +3734,9 @@
       <c r="AA27" s="2" t="n">
         <v>17145</v>
       </c>
+      <c r="AB27" s="2" t="n">
+        <v>17237</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -3739,6 +3820,9 @@
       <c r="AA28" s="2" t="n">
         <v>30685</v>
       </c>
+      <c r="AB28" s="2" t="n">
+        <v>31120</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -3822,6 +3906,9 @@
       <c r="AA29" s="2" t="n">
         <v>12552</v>
       </c>
+      <c r="AB29" s="2" t="n">
+        <v>12600</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -3905,6 +3992,9 @@
       <c r="AA30" s="2" t="n">
         <v>7040</v>
       </c>
+      <c r="AB30" s="2" t="n">
+        <v>7099</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -3988,6 +4078,9 @@
       <c r="AA31" s="2" t="n">
         <v>4433</v>
       </c>
+      <c r="AB31" s="2" t="n">
+        <v>4486</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -4071,6 +4164,9 @@
       <c r="AA32" s="2" t="n">
         <v>1476</v>
       </c>
+      <c r="AB32" s="2" t="n">
+        <v>1492</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -4154,6 +4250,9 @@
       <c r="AA33" s="2" t="n">
         <v>1997</v>
       </c>
+      <c r="AB33" s="2" t="n">
+        <v>2009</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -4237,6 +4336,9 @@
       <c r="AA34" s="2" t="n">
         <v>1735</v>
       </c>
+      <c r="AB34" s="2" t="n">
+        <v>1753</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -4320,6 +4422,9 @@
       <c r="AA35" s="2" t="n">
         <v>786</v>
       </c>
+      <c r="AB35" s="2" t="n">
+        <v>794</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -4403,6 +4508,9 @@
       <c r="AA36" s="2" t="n">
         <v>4668</v>
       </c>
+      <c r="AB36" s="2" t="n">
+        <v>4720</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -4486,6 +4594,9 @@
       <c r="AA37" s="2" t="n">
         <v>3611</v>
       </c>
+      <c r="AB37" s="2" t="n">
+        <v>3640</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -4569,6 +4680,9 @@
       <c r="AA38" s="2" t="n">
         <v>11286</v>
       </c>
+      <c r="AB38" s="2" t="n">
+        <v>11365</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -4652,6 +4766,9 @@
       <c r="AA39" s="2" t="n">
         <v>5222</v>
       </c>
+      <c r="AB39" s="2" t="n">
+        <v>5250</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -4735,6 +4852,9 @@
       <c r="AA40" s="2" t="n">
         <v>2158</v>
       </c>
+      <c r="AB40" s="2" t="n">
+        <v>2172</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -4818,6 +4938,9 @@
       <c r="AA41" s="2" t="n">
         <v>30202</v>
       </c>
+      <c r="AB41" s="2" t="n">
+        <v>30347</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -4901,6 +5024,9 @@
       <c r="AA42" s="2" t="n">
         <v>1665</v>
       </c>
+      <c r="AB42" s="2" t="n">
+        <v>1676</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -4984,6 +5110,9 @@
       <c r="AA43" s="2" t="n">
         <v>7282</v>
       </c>
+      <c r="AB43" s="2" t="n">
+        <v>7342</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -5067,6 +5196,9 @@
       <c r="AA44" s="2" t="n">
         <v>6871</v>
       </c>
+      <c r="AB44" s="2" t="n">
+        <v>6930</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -5150,6 +5282,9 @@
       <c r="AA45" s="2" t="n">
         <v>1738</v>
       </c>
+      <c r="AB45" s="2" t="n">
+        <v>1748</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -5233,6 +5368,9 @@
       <c r="AA46" s="2" t="n">
         <v>553</v>
       </c>
+      <c r="AB46" s="2" t="n">
+        <v>558</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -5316,6 +5454,9 @@
       <c r="AA47" s="2" t="n">
         <v>15711</v>
       </c>
+      <c r="AB47" s="2" t="n">
+        <v>15879</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -5399,6 +5540,9 @@
       <c r="AA48" s="2" t="n">
         <v>17350</v>
       </c>
+      <c r="AB48" s="2" t="n">
+        <v>17411</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -5482,6 +5626,9 @@
       <c r="AA49" s="2" t="n">
         <v>5354</v>
       </c>
+      <c r="AB49" s="2" t="n">
+        <v>5414</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -5565,6 +5712,9 @@
       <c r="AA50" s="2" t="n">
         <v>5104</v>
       </c>
+      <c r="AB50" s="2" t="n">
+        <v>5160</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
@@ -5648,6 +5798,9 @@
       <c r="AA51" s="2" t="n">
         <v>496</v>
       </c>
+      <c r="AB51" s="2" t="n">
+        <v>498</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -5731,6 +5884,9 @@
       <c r="AA52" s="2" t="n">
         <v>891</v>
       </c>
+      <c r="AB52" s="2" t="n">
+        <v>899</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -5814,6 +5970,9 @@
       <c r="AA53" s="2" t="n">
         <v>1351</v>
       </c>
+      <c r="AB53" s="2" t="n">
+        <v>1377</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -5897,6 +6056,9 @@
       <c r="AA54" s="2" t="n">
         <v>22415</v>
       </c>
+      <c r="AB54" s="2" t="n">
+        <v>22347</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
@@ -5980,6 +6142,9 @@
       <c r="AA55" s="2" t="n">
         <v>2408</v>
       </c>
+      <c r="AB55" s="2" t="n">
+        <v>2421</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -6063,6 +6228,9 @@
       <c r="AA56" s="2" t="n">
         <v>23280</v>
       </c>
+      <c r="AB56" s="2" t="n">
+        <v>23451</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -6146,6 +6314,9 @@
       <c r="AA57" s="2" t="n">
         <v>21029</v>
       </c>
+      <c r="AB57" s="2" t="n">
+        <v>21198</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -6229,6 +6400,9 @@
       <c r="AA58" s="2" t="n">
         <v>31754</v>
       </c>
+      <c r="AB58" s="2" t="n">
+        <v>32049</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
@@ -6312,6 +6486,9 @@
       <c r="AA59" s="2" t="n">
         <v>3187</v>
       </c>
+      <c r="AB59" s="2" t="n">
+        <v>3224</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -6395,6 +6572,9 @@
       <c r="AA60" s="2" t="n">
         <v>35605</v>
       </c>
+      <c r="AB60" s="2" t="n">
+        <v>36074</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -6478,6 +6658,9 @@
       <c r="AA61" s="2" t="n">
         <v>12921</v>
       </c>
+      <c r="AB61" s="2" t="n">
+        <v>12956</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -6561,6 +6744,9 @@
       <c r="AA62" s="2" t="n">
         <v>5508</v>
       </c>
+      <c r="AB62" s="2" t="n">
+        <v>5587</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
@@ -6644,6 +6830,9 @@
       <c r="AA63" s="2" t="n">
         <v>20382</v>
       </c>
+      <c r="AB63" s="2" t="n">
+        <v>20671</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
@@ -6727,6 +6916,9 @@
       <c r="AA64" s="2" t="n">
         <v>9015</v>
       </c>
+      <c r="AB64" s="2" t="n">
+        <v>9129</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
@@ -6810,6 +7002,9 @@
       <c r="AA65" s="2" t="n">
         <v>10139</v>
       </c>
+      <c r="AB65" s="2" t="n">
+        <v>10263</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
@@ -6893,6 +7088,9 @@
       <c r="AA66" s="2" t="n">
         <v>3197</v>
       </c>
+      <c r="AB66" s="2" t="n">
+        <v>3247</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
@@ -6976,6 +7174,9 @@
       <c r="AA67" s="2" t="n">
         <v>13263</v>
       </c>
+      <c r="AB67" s="2" t="n">
+        <v>13325</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
@@ -7059,6 +7260,9 @@
       <c r="AA68" s="2" t="n">
         <v>12902</v>
       </c>
+      <c r="AB68" s="2" t="n">
+        <v>13069</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
@@ -7142,6 +7346,9 @@
       <c r="AA69" s="2" t="n">
         <v>5924</v>
       </c>
+      <c r="AB69" s="2" t="n">
+        <v>6003</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
@@ -7225,6 +7432,9 @@
       <c r="AA70" s="2" t="n">
         <v>23151</v>
       </c>
+      <c r="AB70" s="2" t="n">
+        <v>23455</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
@@ -7308,6 +7518,9 @@
       <c r="AA71" s="2" t="n">
         <v>40628</v>
       </c>
+      <c r="AB71" s="2" t="n">
+        <v>41306</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
@@ -7391,6 +7604,9 @@
       <c r="AA72" s="2" t="n">
         <v>18591</v>
       </c>
+      <c r="AB72" s="2" t="n">
+        <v>18631</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
@@ -7474,6 +7690,9 @@
       <c r="AA73" s="2" t="n">
         <v>8555</v>
       </c>
+      <c r="AB73" s="2" t="n">
+        <v>8643</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
@@ -7557,6 +7776,9 @@
       <c r="AA74" s="2" t="n">
         <v>12013</v>
       </c>
+      <c r="AB74" s="2" t="n">
+        <v>12149</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
@@ -7640,6 +7862,9 @@
       <c r="AA75" s="2" t="n">
         <v>24657</v>
       </c>
+      <c r="AB75" s="2" t="n">
+        <v>24907</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
@@ -7723,6 +7948,9 @@
       <c r="AA76" s="2" t="n">
         <v>8495</v>
       </c>
+      <c r="AB76" s="2" t="n">
+        <v>8602</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
@@ -7806,6 +8034,9 @@
       <c r="AA77" s="2" t="n">
         <v>9435</v>
       </c>
+      <c r="AB77" s="2" t="n">
+        <v>9475</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
@@ -7889,6 +8120,9 @@
       <c r="AA78" s="2" t="n">
         <v>2666</v>
       </c>
+      <c r="AB78" s="2" t="n">
+        <v>2685</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
@@ -7972,6 +8206,9 @@
       <c r="AA79" s="2" t="n">
         <v>5255</v>
       </c>
+      <c r="AB79" s="2" t="n">
+        <v>5308</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
@@ -8055,6 +8292,9 @@
       <c r="AA80" s="2" t="n">
         <v>2104</v>
       </c>
+      <c r="AB80" s="2" t="n">
+        <v>2121</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
@@ -8138,6 +8378,9 @@
       <c r="AA81" s="2" t="n">
         <v>2654</v>
       </c>
+      <c r="AB81" s="2" t="n">
+        <v>2668</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
@@ -8221,6 +8464,9 @@
       <c r="AA82" s="2" t="n">
         <v>25919</v>
       </c>
+      <c r="AB82" s="2" t="n">
+        <v>25866</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
@@ -8304,6 +8550,9 @@
       <c r="AA83" s="2" t="n">
         <v>8513</v>
       </c>
+      <c r="AB83" s="2" t="n">
+        <v>8617</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
@@ -8387,6 +8636,9 @@
       <c r="AA84" s="2" t="n">
         <v>12850</v>
       </c>
+      <c r="AB84" s="2" t="n">
+        <v>12913</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
@@ -8470,6 +8722,9 @@
       <c r="AA85" s="2" t="n">
         <v>20233</v>
       </c>
+      <c r="AB85" s="2" t="n">
+        <v>20551</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
@@ -8553,6 +8808,9 @@
       <c r="AA86" s="2" t="n">
         <v>17971</v>
       </c>
+      <c r="AB86" s="2" t="n">
+        <v>18118</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
@@ -8636,6 +8894,9 @@
       <c r="AA87" s="2" t="n">
         <v>32098</v>
       </c>
+      <c r="AB87" s="2" t="n">
+        <v>32041</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
@@ -8719,6 +8980,9 @@
       <c r="AA88" s="2" t="n">
         <v>7385</v>
       </c>
+      <c r="AB88" s="2" t="n">
+        <v>7463</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
@@ -8802,6 +9066,9 @@
       <c r="AA89" s="2" t="n">
         <v>23495</v>
       </c>
+      <c r="AB89" s="2" t="n">
+        <v>23755</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
@@ -8885,6 +9152,9 @@
       <c r="AA90" s="2" t="n">
         <v>28945</v>
       </c>
+      <c r="AB90" s="2" t="n">
+        <v>28844</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
@@ -8968,6 +9238,9 @@
       <c r="AA91" s="2" t="n">
         <v>14011</v>
       </c>
+      <c r="AB91" s="2" t="n">
+        <v>14082</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
@@ -9051,6 +9324,9 @@
       <c r="AA92" s="2" t="n">
         <v>6063</v>
       </c>
+      <c r="AB92" s="2" t="n">
+        <v>6086</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
@@ -9134,6 +9410,9 @@
       <c r="AA93" s="2" t="n">
         <v>13694</v>
       </c>
+      <c r="AB93" s="2" t="n">
+        <v>13832</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
@@ -9217,6 +9496,9 @@
       <c r="AA94" s="2" t="n">
         <v>1566</v>
       </c>
+      <c r="AB94" s="2" t="n">
+        <v>1573</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
@@ -9300,6 +9582,9 @@
       <c r="AA95" s="2" t="n">
         <v>852</v>
       </c>
+      <c r="AB95" s="2" t="n">
+        <v>861</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
@@ -9383,6 +9668,9 @@
       <c r="AA96" s="2" t="n">
         <v>1526</v>
       </c>
+      <c r="AB96" s="2" t="n">
+        <v>1546</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
@@ -9466,6 +9754,9 @@
       <c r="AA97" s="2" t="n">
         <v>709</v>
       </c>
+      <c r="AB97" s="2" t="n">
+        <v>721</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
@@ -9549,6 +9840,9 @@
       <c r="AA98" s="2" t="n">
         <v>2298</v>
       </c>
+      <c r="AB98" s="2" t="n">
+        <v>2330</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
@@ -9632,6 +9926,9 @@
       <c r="AA99" s="2" t="n">
         <v>5216</v>
       </c>
+      <c r="AB99" s="2" t="n">
+        <v>5251</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
@@ -9715,6 +10012,9 @@
       <c r="AA100" s="2" t="n">
         <v>702</v>
       </c>
+      <c r="AB100" s="2" t="n">
+        <v>702</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
@@ -9798,6 +10098,9 @@
       <c r="AA101" s="2" t="n">
         <v>2082</v>
       </c>
+      <c r="AB101" s="2" t="n">
+        <v>2088</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
@@ -9881,6 +10184,9 @@
       <c r="AA102" s="2" t="n">
         <v>32617</v>
       </c>
+      <c r="AB102" s="2" t="n">
+        <v>32605</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="n">
@@ -9964,6 +10270,9 @@
       <c r="AA103" s="2" t="n">
         <v>19011</v>
       </c>
+      <c r="AB103" s="2" t="n">
+        <v>19207</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
@@ -10047,6 +10356,9 @@
       <c r="AA104" s="2" t="n">
         <v>6784</v>
       </c>
+      <c r="AB104" s="2" t="n">
+        <v>6833</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="n">
@@ -10130,6 +10442,9 @@
       <c r="AA105" s="2" t="n">
         <v>21730</v>
       </c>
+      <c r="AB105" s="2" t="n">
+        <v>22032</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
@@ -10213,6 +10528,9 @@
       <c r="AA106" s="2" t="n">
         <v>48345</v>
       </c>
+      <c r="AB106" s="2" t="n">
+        <v>48435</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
@@ -10296,6 +10614,9 @@
       <c r="AA107" s="2" t="n">
         <v>6867</v>
       </c>
+      <c r="AB107" s="2" t="n">
+        <v>6873</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
@@ -10379,6 +10700,9 @@
       <c r="AA108" s="2" t="n">
         <v>35523</v>
       </c>
+      <c r="AB108" s="2" t="n">
+        <v>35584</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="n">
@@ -10462,6 +10786,9 @@
       <c r="AA109" s="2" t="n">
         <v>7310</v>
       </c>
+      <c r="AB109" s="2" t="n">
+        <v>7318</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
@@ -10545,6 +10872,9 @@
       <c r="AA110" s="2" t="n">
         <v>9389</v>
       </c>
+      <c r="AB110" s="2" t="n">
+        <v>9344</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
@@ -10628,6 +10958,9 @@
       <c r="AA111" s="2" t="n">
         <v>7513</v>
       </c>
+      <c r="AB111" s="2" t="n">
+        <v>7497</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
@@ -10711,6 +11044,9 @@
       <c r="AA112" s="2" t="n">
         <v>8028</v>
       </c>
+      <c r="AB112" s="2" t="n">
+        <v>7972</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
@@ -10794,6 +11130,9 @@
       <c r="AA113" s="2" t="n">
         <v>9059</v>
       </c>
+      <c r="AB113" s="2" t="n">
+        <v>9045</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
@@ -10877,6 +11216,9 @@
       <c r="AA114" s="2" t="n">
         <v>2848</v>
       </c>
+      <c r="AB114" s="2" t="n">
+        <v>2854</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="n">
@@ -10960,6 +11302,9 @@
       <c r="AA115" s="2" t="n">
         <v>3485</v>
       </c>
+      <c r="AB115" s="2" t="n">
+        <v>3495</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
@@ -11043,6 +11388,9 @@
       <c r="AA116" s="2" t="n">
         <v>4855</v>
       </c>
+      <c r="AB116" s="2" t="n">
+        <v>4865</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
@@ -11126,6 +11474,9 @@
       <c r="AA117" s="2" t="n">
         <v>4629</v>
       </c>
+      <c r="AB117" s="2" t="n">
+        <v>4663</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
@@ -11209,6 +11560,9 @@
       <c r="AA118" s="2" t="n">
         <v>1734</v>
       </c>
+      <c r="AB118" s="2" t="n">
+        <v>1746</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
@@ -11292,6 +11646,9 @@
       <c r="AA119" s="2" t="n">
         <v>2252</v>
       </c>
+      <c r="AB119" s="2" t="n">
+        <v>2269</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="n">
@@ -11375,6 +11732,9 @@
       <c r="AA120" s="2" t="n">
         <v>1854</v>
       </c>
+      <c r="AB120" s="2" t="n">
+        <v>1870</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="n">
@@ -11458,6 +11818,9 @@
       <c r="AA121" s="2" t="n">
         <v>2142</v>
       </c>
+      <c r="AB121" s="2" t="n">
+        <v>2164</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="n">
@@ -11541,6 +11904,9 @@
       <c r="AA122" s="2" t="n">
         <v>1263</v>
       </c>
+      <c r="AB122" s="2" t="n">
+        <v>1278</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="n">
@@ -11624,6 +11990,9 @@
       <c r="AA123" s="2" t="n">
         <v>48214</v>
       </c>
+      <c r="AB123" s="2" t="n">
+        <v>48326</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="n">
@@ -11707,6 +12076,9 @@
       <c r="AA124" s="2" t="n">
         <v>52020</v>
       </c>
+      <c r="AB124" s="2" t="n">
+        <v>52686</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="n">
@@ -11790,6 +12162,9 @@
       <c r="AA125" s="2" t="n">
         <v>8870</v>
       </c>
+      <c r="AB125" s="2" t="n">
+        <v>9002</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="n">
@@ -11873,6 +12248,9 @@
       <c r="AA126" s="2" t="n">
         <v>31220</v>
       </c>
+      <c r="AB126" s="2" t="n">
+        <v>31637</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="n">
@@ -11956,6 +12334,9 @@
       <c r="AA127" s="2" t="n">
         <v>26236</v>
       </c>
+      <c r="AB127" s="2" t="n">
+        <v>26642</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="n">
@@ -12039,6 +12420,9 @@
       <c r="AA128" s="2" t="n">
         <v>22265</v>
       </c>
+      <c r="AB128" s="2" t="n">
+        <v>22586</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="n">
@@ -12122,6 +12506,9 @@
       <c r="AA129" s="2" t="n">
         <v>12193</v>
       </c>
+      <c r="AB129" s="2" t="n">
+        <v>12396</v>
+      </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="n">
@@ -12205,6 +12592,9 @@
       <c r="AA130" s="2" t="n">
         <v>33733</v>
       </c>
+      <c r="AB130" s="2" t="n">
+        <v>34182</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="n">
@@ -12288,6 +12678,9 @@
       <c r="AA131" s="2" t="n">
         <v>13395</v>
       </c>
+      <c r="AB131" s="2" t="n">
+        <v>13561</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="n">
@@ -12371,6 +12764,9 @@
       <c r="AA132" s="2" t="n">
         <v>33192</v>
       </c>
+      <c r="AB132" s="2" t="n">
+        <v>33654</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="n">
@@ -12454,6 +12850,9 @@
       <c r="AA133" s="2" t="n">
         <v>9282</v>
       </c>
+      <c r="AB133" s="2" t="n">
+        <v>9349</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="n">
@@ -12537,6 +12936,9 @@
       <c r="AA134" s="2" t="n">
         <v>14123</v>
       </c>
+      <c r="AB134" s="2" t="n">
+        <v>14338</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="n">
@@ -12620,6 +13022,9 @@
       <c r="AA135" s="2" t="n">
         <v>9376</v>
       </c>
+      <c r="AB135" s="2" t="n">
+        <v>9492</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="n">
@@ -12703,6 +13108,9 @@
       <c r="AA136" s="2" t="n">
         <v>3968</v>
       </c>
+      <c r="AB136" s="2" t="n">
+        <v>4021</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="n">
@@ -12786,6 +13194,9 @@
       <c r="AA137" s="2" t="n">
         <v>9106</v>
       </c>
+      <c r="AB137" s="2" t="n">
+        <v>9107</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="n">
@@ -12869,6 +13280,9 @@
       <c r="AA138" s="2" t="n">
         <v>5620</v>
       </c>
+      <c r="AB138" s="2" t="n">
+        <v>5699</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="n">
@@ -12952,6 +13366,9 @@
       <c r="AA139" s="2" t="n">
         <v>13264</v>
       </c>
+      <c r="AB139" s="2" t="n">
+        <v>13406</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="n">
@@ -13035,6 +13452,9 @@
       <c r="AA140" s="2" t="n">
         <v>9465</v>
       </c>
+      <c r="AB140" s="2" t="n">
+        <v>9564</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="n">
@@ -13118,6 +13538,9 @@
       <c r="AA141" s="2" t="n">
         <v>4553</v>
       </c>
+      <c r="AB141" s="2" t="n">
+        <v>4603</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="n">
@@ -13201,6 +13624,9 @@
       <c r="AA142" s="2" t="n">
         <v>10783</v>
       </c>
+      <c r="AB142" s="2" t="n">
+        <v>10904</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="n">
@@ -13284,6 +13710,9 @@
       <c r="AA143" s="2" t="n">
         <v>5869</v>
       </c>
+      <c r="AB143" s="2" t="n">
+        <v>5938</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="n">
@@ -13367,6 +13796,9 @@
       <c r="AA144" s="2" t="n">
         <v>9697</v>
       </c>
+      <c r="AB144" s="2" t="n">
+        <v>9793</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="n">
@@ -13450,6 +13882,9 @@
       <c r="AA145" s="2" t="n">
         <v>8308</v>
       </c>
+      <c r="AB145" s="2" t="n">
+        <v>8402</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="n">
@@ -13533,6 +13968,9 @@
       <c r="AA146" s="2" t="n">
         <v>2698</v>
       </c>
+      <c r="AB146" s="2" t="n">
+        <v>2727</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="n">
@@ -13616,6 +14054,9 @@
       <c r="AA147" s="2" t="n">
         <v>2753</v>
       </c>
+      <c r="AB147" s="2" t="n">
+        <v>2765</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="n">
@@ -13699,6 +14140,9 @@
       <c r="AA148" s="2" t="n">
         <v>515</v>
       </c>
+      <c r="AB148" s="2" t="n">
+        <v>515</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="n">
@@ -13782,6 +14226,9 @@
       <c r="AA149" s="2" t="n">
         <v>12212</v>
       </c>
+      <c r="AB149" s="2" t="n">
+        <v>12371</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="n">
@@ -13865,6 +14312,9 @@
       <c r="AA150" s="2" t="n">
         <v>16126</v>
       </c>
+      <c r="AB150" s="2" t="n">
+        <v>16146</v>
+      </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="n">
@@ -13948,6 +14398,9 @@
       <c r="AA151" s="2" t="n">
         <v>7210</v>
       </c>
+      <c r="AB151" s="2" t="n">
+        <v>7293</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
@@ -14031,6 +14484,9 @@
       <c r="AA152" s="2" t="n">
         <v>10101</v>
       </c>
+      <c r="AB152" s="2" t="n">
+        <v>10231</v>
+      </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="n">
@@ -14114,6 +14570,9 @@
       <c r="AA153" s="2" t="n">
         <v>13505</v>
       </c>
+      <c r="AB153" s="2" t="n">
+        <v>13660</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="n">
@@ -14197,6 +14656,9 @@
       <c r="AA154" s="2" t="n">
         <v>9922</v>
       </c>
+      <c r="AB154" s="2" t="n">
+        <v>10050</v>
+      </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="n">
@@ -14280,6 +14742,9 @@
       <c r="AA155" s="2" t="n">
         <v>13103</v>
       </c>
+      <c r="AB155" s="2" t="n">
+        <v>13274</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="n">
@@ -14363,6 +14828,9 @@
       <c r="AA156" s="2" t="n">
         <v>8905</v>
       </c>
+      <c r="AB156" s="2" t="n">
+        <v>9018</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="n">
@@ -14446,6 +14914,9 @@
       <c r="AA157" s="2" t="n">
         <v>3058</v>
       </c>
+      <c r="AB157" s="2" t="n">
+        <v>3071</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="n">
@@ -14529,6 +15000,9 @@
       <c r="AA158" s="2" t="n">
         <v>1187</v>
       </c>
+      <c r="AB158" s="2" t="n">
+        <v>1201</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="n">
@@ -14612,6 +15086,9 @@
       <c r="AA159" s="2" t="n">
         <v>1496</v>
       </c>
+      <c r="AB159" s="2" t="n">
+        <v>1517</v>
+      </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="n">
@@ -14695,6 +15172,9 @@
       <c r="AA160" s="2" t="n">
         <v>1467</v>
       </c>
+      <c r="AB160" s="2" t="n">
+        <v>1487</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="n">
@@ -14778,6 +15258,9 @@
       <c r="AA161" s="2" t="n">
         <v>7995</v>
       </c>
+      <c r="AB161" s="2" t="n">
+        <v>8015</v>
+      </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="n">
@@ -14861,6 +15344,9 @@
       <c r="AA162" s="2" t="n">
         <v>4348</v>
       </c>
+      <c r="AB162" s="2" t="n">
+        <v>4396</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="n">
@@ -14944,6 +15430,9 @@
       <c r="AA163" s="2" t="n">
         <v>3786</v>
       </c>
+      <c r="AB163" s="2" t="n">
+        <v>3832</v>
+      </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="n">
@@ -15027,6 +15516,9 @@
       <c r="AA164" s="2" t="n">
         <v>3476</v>
       </c>
+      <c r="AB164" s="2" t="n">
+        <v>3521</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="n">
@@ -15110,6 +15602,9 @@
       <c r="AA165" s="2" t="n">
         <v>4208</v>
       </c>
+      <c r="AB165" s="2" t="n">
+        <v>4261</v>
+      </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="n">
@@ -15193,6 +15688,9 @@
       <c r="AA166" s="2" t="n">
         <v>2304</v>
       </c>
+      <c r="AB166" s="2" t="n">
+        <v>2326</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="n">
@@ -15276,6 +15774,9 @@
       <c r="AA167" s="2" t="n">
         <v>2482</v>
       </c>
+      <c r="AB167" s="2" t="n">
+        <v>2510</v>
+      </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="n">
@@ -15359,6 +15860,9 @@
       <c r="AA168" s="2" t="n">
         <v>1011</v>
       </c>
+      <c r="AB168" s="2" t="n">
+        <v>1019</v>
+      </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="n">
@@ -15442,6 +15946,9 @@
       <c r="AA169" s="2" t="n">
         <v>17273</v>
       </c>
+      <c r="AB169" s="2" t="n">
+        <v>17348</v>
+      </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="n">
@@ -15525,6 +16032,9 @@
       <c r="AA170" s="2" t="n">
         <v>5701</v>
       </c>
+      <c r="AB170" s="2" t="n">
+        <v>5782</v>
+      </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="n">
@@ -15608,6 +16118,9 @@
       <c r="AA171" s="2" t="n">
         <v>3637</v>
       </c>
+      <c r="AB171" s="2" t="n">
+        <v>3666</v>
+      </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="n">
@@ -15691,6 +16204,9 @@
       <c r="AA172" s="2" t="n">
         <v>5465</v>
       </c>
+      <c r="AB172" s="2" t="n">
+        <v>5533</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="n">
@@ -15774,6 +16290,9 @@
       <c r="AA173" s="2" t="n">
         <v>4019</v>
       </c>
+      <c r="AB173" s="2" t="n">
+        <v>4076</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="n">
@@ -15857,6 +16376,9 @@
       <c r="AA174" s="2" t="n">
         <v>3646</v>
       </c>
+      <c r="AB174" s="2" t="n">
+        <v>3688</v>
+      </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="n">
@@ -15940,6 +16462,9 @@
       <c r="AA175" s="2" t="n">
         <v>4571</v>
       </c>
+      <c r="AB175" s="2" t="n">
+        <v>4638</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="n">
@@ -16023,6 +16548,9 @@
       <c r="AA176" s="2" t="n">
         <v>4976</v>
       </c>
+      <c r="AB176" s="2" t="n">
+        <v>5033</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="n">
@@ -16106,6 +16634,9 @@
       <c r="AA177" s="2" t="n">
         <v>3766</v>
       </c>
+      <c r="AB177" s="2" t="n">
+        <v>3764</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="n">
@@ -16189,6 +16720,9 @@
       <c r="AA178" s="2" t="n">
         <v>9792</v>
       </c>
+      <c r="AB178" s="2" t="n">
+        <v>9901</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="n">
@@ -16272,6 +16806,9 @@
       <c r="AA179" s="2" t="n">
         <v>8844</v>
       </c>
+      <c r="AB179" s="2" t="n">
+        <v>8931</v>
+      </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="n">
@@ -16355,6 +16892,9 @@
       <c r="AA180" s="2" t="n">
         <v>3339</v>
       </c>
+      <c r="AB180" s="2" t="n">
+        <v>3379</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="n">
@@ -16438,6 +16978,9 @@
       <c r="AA181" s="2" t="n">
         <v>2430</v>
       </c>
+      <c r="AB181" s="2" t="n">
+        <v>2457</v>
+      </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="n">
@@ -16521,6 +17064,9 @@
       <c r="AA182" s="2" t="n">
         <v>8320</v>
       </c>
+      <c r="AB182" s="2" t="n">
+        <v>8435</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="n">
@@ -16604,6 +17150,9 @@
       <c r="AA183" s="2" t="n">
         <v>4885</v>
       </c>
+      <c r="AB183" s="2" t="n">
+        <v>4938</v>
+      </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="n">
@@ -16687,6 +17236,9 @@
       <c r="AA184" s="2" t="n">
         <v>8200</v>
       </c>
+      <c r="AB184" s="2" t="n">
+        <v>8243</v>
+      </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="n">
@@ -16770,6 +17322,9 @@
       <c r="AA185" s="2" t="n">
         <v>5564</v>
       </c>
+      <c r="AB185" s="2" t="n">
+        <v>5647</v>
+      </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="n">
@@ -16853,6 +17408,9 @@
       <c r="AA186" s="2" t="n">
         <v>6560</v>
       </c>
+      <c r="AB186" s="2" t="n">
+        <v>6655</v>
+      </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="n">
@@ -16936,6 +17494,9 @@
       <c r="AA187" s="2" t="n">
         <v>11148</v>
       </c>
+      <c r="AB187" s="2" t="n">
+        <v>11330</v>
+      </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="n">
@@ -17019,6 +17580,9 @@
       <c r="AA188" s="2" t="n">
         <v>2998</v>
       </c>
+      <c r="AB188" s="2" t="n">
+        <v>3051</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="n">
@@ -17102,6 +17666,9 @@
       <c r="AA189" s="2" t="n">
         <v>10591</v>
       </c>
+      <c r="AB189" s="2" t="n">
+        <v>10680</v>
+      </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="n">
@@ -17185,6 +17752,9 @@
       <c r="AA190" s="2" t="n">
         <v>2213</v>
       </c>
+      <c r="AB190" s="2" t="n">
+        <v>2249</v>
+      </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="n">
@@ -17268,6 +17838,9 @@
       <c r="AA191" s="2" t="n">
         <v>1225</v>
       </c>
+      <c r="AB191" s="2" t="n">
+        <v>1242</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="n">
@@ -17351,6 +17924,9 @@
       <c r="AA192" s="2" t="n">
         <v>7538</v>
       </c>
+      <c r="AB192" s="2" t="n">
+        <v>7685</v>
+      </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="n">
@@ -17434,6 +18010,9 @@
       <c r="AA193" s="2" t="n">
         <v>2539</v>
       </c>
+      <c r="AB193" s="2" t="n">
+        <v>2592</v>
+      </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="n">
@@ -17517,6 +18096,9 @@
       <c r="AA194" s="2" t="n">
         <v>45859</v>
       </c>
+      <c r="AB194" s="2" t="n">
+        <v>46127</v>
+      </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="n">
@@ -17600,6 +18182,9 @@
       <c r="AA195" s="2" t="n">
         <v>18294</v>
       </c>
+      <c r="AB195" s="2" t="n">
+        <v>18517</v>
+      </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="n">
@@ -17683,6 +18268,9 @@
       <c r="AA196" s="2" t="n">
         <v>408</v>
       </c>
+      <c r="AB196" s="2" t="n">
+        <v>420</v>
+      </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="n">
@@ -17766,6 +18354,9 @@
       <c r="AA197" s="2" t="n">
         <v>25843</v>
       </c>
+      <c r="AB197" s="2" t="n">
+        <v>26305</v>
+      </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="n">
@@ -17849,6 +18440,9 @@
       <c r="AA198" s="2" t="n">
         <v>11975</v>
       </c>
+      <c r="AB198" s="2" t="n">
+        <v>12172</v>
+      </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="n">
@@ -17932,6 +18526,9 @@
       <c r="AA199" s="2" t="n">
         <v>24747</v>
       </c>
+      <c r="AB199" s="2" t="n">
+        <v>25359</v>
+      </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="n">
@@ -18015,6 +18612,9 @@
       <c r="AA200" s="2" t="n">
         <v>19297</v>
       </c>
+      <c r="AB200" s="2" t="n">
+        <v>19584</v>
+      </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="n">
@@ -18098,6 +18698,9 @@
       <c r="AA201" s="2" t="n">
         <v>7865</v>
       </c>
+      <c r="AB201" s="2" t="n">
+        <v>7964</v>
+      </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="n">
@@ -18181,6 +18784,9 @@
       <c r="AA202" s="2" t="n">
         <v>7828</v>
       </c>
+      <c r="AB202" s="2" t="n">
+        <v>7940</v>
+      </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="n">
@@ -18264,6 +18870,9 @@
       <c r="AA203" s="2" t="n">
         <v>2156</v>
       </c>
+      <c r="AB203" s="2" t="n">
+        <v>2173</v>
+      </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="n">
@@ -18347,6 +18956,9 @@
       <c r="AA204" s="2" t="n">
         <v>15183</v>
       </c>
+      <c r="AB204" s="2" t="n">
+        <v>15537</v>
+      </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="n">
@@ -18430,6 +19042,9 @@
       <c r="AA205" s="2" t="n">
         <v>4273</v>
       </c>
+      <c r="AB205" s="2" t="n">
+        <v>4321</v>
+      </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="n">
@@ -18513,6 +19128,9 @@
       <c r="AA206" s="2" t="n">
         <v>19421</v>
       </c>
+      <c r="AB206" s="2" t="n">
+        <v>19696</v>
+      </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="n">
@@ -18596,6 +19214,9 @@
       <c r="AA207" s="2" t="n">
         <v>4378</v>
       </c>
+      <c r="AB207" s="2" t="n">
+        <v>4397</v>
+      </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="n">
@@ -18679,6 +19300,9 @@
       <c r="AA208" s="2" t="n">
         <v>2011</v>
       </c>
+      <c r="AB208" s="2" t="n">
+        <v>2031</v>
+      </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="n">
@@ -18762,6 +19386,9 @@
       <c r="AA209" s="2" t="n">
         <v>1563</v>
       </c>
+      <c r="AB209" s="2" t="n">
+        <v>1582</v>
+      </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="n">
@@ -18845,6 +19472,9 @@
       <c r="AA210" s="2" t="n">
         <v>1409</v>
       </c>
+      <c r="AB210" s="2" t="n">
+        <v>1427</v>
+      </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="n">
@@ -18928,6 +19558,9 @@
       <c r="AA211" s="2" t="n">
         <v>1691</v>
       </c>
+      <c r="AB211" s="2" t="n">
+        <v>1712</v>
+      </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="n">
@@ -19011,6 +19644,9 @@
       <c r="AA212" s="2" t="n">
         <v>932</v>
       </c>
+      <c r="AB212" s="2" t="n">
+        <v>944</v>
+      </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="n">
@@ -19094,6 +19730,9 @@
       <c r="AA213" s="2" t="n">
         <v>2505</v>
       </c>
+      <c r="AB213" s="2" t="n">
+        <v>2536</v>
+      </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="n">
@@ -19177,6 +19816,9 @@
       <c r="AA214" s="2" t="n">
         <v>8339</v>
       </c>
+      <c r="AB214" s="2" t="n">
+        <v>8382</v>
+      </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="n">
@@ -19260,6 +19902,9 @@
       <c r="AA215" s="2" t="n">
         <v>6466</v>
       </c>
+      <c r="AB215" s="2" t="n">
+        <v>6539</v>
+      </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="n">
@@ -19343,6 +19988,9 @@
       <c r="AA216" s="2" t="n">
         <v>379</v>
       </c>
+      <c r="AB216" s="2" t="n">
+        <v>380</v>
+      </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="n">
@@ -19426,6 +20074,9 @@
       <c r="AA217" s="2" t="n">
         <v>4412</v>
       </c>
+      <c r="AB217" s="2" t="n">
+        <v>4463</v>
+      </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="n">
@@ -19509,6 +20160,9 @@
       <c r="AA218" s="2" t="n">
         <v>2796</v>
       </c>
+      <c r="AB218" s="2" t="n">
+        <v>2832</v>
+      </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="n">
@@ -19592,6 +20246,9 @@
       <c r="AA219" s="2" t="n">
         <v>16554</v>
       </c>
+      <c r="AB219" s="2" t="n">
+        <v>16850</v>
+      </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="n">
@@ -19675,6 +20332,9 @@
       <c r="AA220" s="2" t="n">
         <v>5692</v>
       </c>
+      <c r="AB220" s="2" t="n">
+        <v>5714</v>
+      </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="n">
@@ -19758,6 +20418,9 @@
       <c r="AA221" s="2" t="n">
         <v>8723</v>
       </c>
+      <c r="AB221" s="2" t="n">
+        <v>8795</v>
+      </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="n">
@@ -19841,6 +20504,9 @@
       <c r="AA222" s="2" t="n">
         <v>5334</v>
       </c>
+      <c r="AB222" s="2" t="n">
+        <v>5363</v>
+      </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="n">
@@ -19924,6 +20590,9 @@
       <c r="AA223" s="2" t="n">
         <v>5428</v>
       </c>
+      <c r="AB223" s="2" t="n">
+        <v>5479</v>
+      </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="n">
@@ -20007,6 +20676,9 @@
       <c r="AA224" s="2" t="n">
         <v>3970</v>
       </c>
+      <c r="AB224" s="2" t="n">
+        <v>4017</v>
+      </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="n">
@@ -20090,6 +20762,9 @@
       <c r="AA225" s="2" t="n">
         <v>4078</v>
       </c>
+      <c r="AB225" s="2" t="n">
+        <v>4129</v>
+      </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="n">
@@ -20173,6 +20848,9 @@
       <c r="AA226" s="2" t="n">
         <v>4987</v>
       </c>
+      <c r="AB226" s="2" t="n">
+        <v>5119</v>
+      </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="n">
@@ -20256,6 +20934,9 @@
       <c r="AA227" s="2" t="n">
         <v>21097</v>
       </c>
+      <c r="AB227" s="2" t="n">
+        <v>21714</v>
+      </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="n">
@@ -20339,6 +21020,9 @@
       <c r="AA228" s="2" t="n">
         <v>2309</v>
       </c>
+      <c r="AB228" s="2" t="n">
+        <v>2333</v>
+      </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="n">
@@ -20422,6 +21106,9 @@
       <c r="AA229" s="2" t="n">
         <v>7690</v>
       </c>
+      <c r="AB229" s="2" t="n">
+        <v>7772</v>
+      </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="n">
@@ -20505,6 +21192,9 @@
       <c r="AA230" s="2" t="n">
         <v>3345</v>
       </c>
+      <c r="AB230" s="2" t="n">
+        <v>3369</v>
+      </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="n">
@@ -20588,6 +21278,9 @@
       <c r="AA231" s="2" t="n">
         <v>9982</v>
       </c>
+      <c r="AB231" s="2" t="n">
+        <v>10117</v>
+      </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="n">
@@ -20671,6 +21364,9 @@
       <c r="AA232" s="2" t="n">
         <v>1967</v>
       </c>
+      <c r="AB232" s="2" t="n">
+        <v>1990</v>
+      </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="n">
@@ -20754,6 +21450,9 @@
       <c r="AA233" s="2" t="n">
         <v>1087</v>
       </c>
+      <c r="AB233" s="2" t="n">
+        <v>1092</v>
+      </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="n">
@@ -20837,6 +21536,9 @@
       <c r="AA234" s="2" t="n">
         <v>6424</v>
       </c>
+      <c r="AB234" s="2" t="n">
+        <v>6497</v>
+      </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="n">
@@ -20920,6 +21622,9 @@
       <c r="AA235" s="2" t="n">
         <v>12351</v>
       </c>
+      <c r="AB235" s="2" t="n">
+        <v>12310</v>
+      </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="n">
@@ -21003,6 +21708,9 @@
       <c r="AA236" s="2" t="n">
         <v>10447</v>
       </c>
+      <c r="AB236" s="2" t="n">
+        <v>10465</v>
+      </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="n">
@@ -21086,6 +21794,9 @@
       <c r="AA237" s="2" t="n">
         <v>19291</v>
       </c>
+      <c r="AB237" s="2" t="n">
+        <v>19390</v>
+      </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="n">
@@ -21169,6 +21880,9 @@
       <c r="AA238" s="2" t="n">
         <v>29662</v>
       </c>
+      <c r="AB238" s="2" t="n">
+        <v>29913</v>
+      </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="n">
@@ -21252,6 +21966,9 @@
       <c r="AA239" s="2" t="n">
         <v>36113</v>
       </c>
+      <c r="AB239" s="2" t="n">
+        <v>36408</v>
+      </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="n">
@@ -21335,6 +22052,9 @@
       <c r="AA240" s="2" t="n">
         <v>16441</v>
       </c>
+      <c r="AB240" s="2" t="n">
+        <v>16547</v>
+      </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="n">
@@ -21418,6 +22138,9 @@
       <c r="AA241" s="2" t="n">
         <v>11989</v>
       </c>
+      <c r="AB241" s="2" t="n">
+        <v>12064</v>
+      </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="n">
@@ -21501,6 +22224,9 @@
       <c r="AA242" s="2" t="n">
         <v>5873</v>
       </c>
+      <c r="AB242" s="2" t="n">
+        <v>5926</v>
+      </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="n">
@@ -21584,6 +22310,9 @@
       <c r="AA243" s="2" t="n">
         <v>11935</v>
       </c>
+      <c r="AB243" s="2" t="n">
+        <v>12004</v>
+      </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="n">
@@ -21667,6 +22396,9 @@
       <c r="AA244" s="2" t="n">
         <v>5068</v>
       </c>
+      <c r="AB244" s="2" t="n">
+        <v>5120</v>
+      </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="n">
@@ -21750,6 +22482,9 @@
       <c r="AA245" s="2" t="n">
         <v>6025</v>
       </c>
+      <c r="AB245" s="2" t="n">
+        <v>6057</v>
+      </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="n">
@@ -21833,6 +22568,9 @@
       <c r="AA246" s="2" t="n">
         <v>21507</v>
       </c>
+      <c r="AB246" s="2" t="n">
+        <v>21561</v>
+      </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="n">
@@ -21916,6 +22654,9 @@
       <c r="AA247" s="2" t="n">
         <v>6439</v>
       </c>
+      <c r="AB247" s="2" t="n">
+        <v>6493</v>
+      </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="n">
@@ -21999,6 +22740,9 @@
       <c r="AA248" s="2" t="n">
         <v>10141</v>
       </c>
+      <c r="AB248" s="2" t="n">
+        <v>10208</v>
+      </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="n">
@@ -22082,6 +22826,9 @@
       <c r="AA249" s="2" t="n">
         <v>5911</v>
       </c>
+      <c r="AB249" s="2" t="n">
+        <v>5944</v>
+      </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="n">
@@ -22165,6 +22912,9 @@
       <c r="AA250" s="2" t="n">
         <v>19378</v>
       </c>
+      <c r="AB250" s="2" t="n">
+        <v>19590</v>
+      </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="n">
@@ -22248,6 +22998,9 @@
       <c r="AA251" s="2" t="n">
         <v>9316</v>
       </c>
+      <c r="AB251" s="2" t="n">
+        <v>9298</v>
+      </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="n">
@@ -22331,6 +23084,9 @@
       <c r="AA252" s="2" t="n">
         <v>25104</v>
       </c>
+      <c r="AB252" s="2" t="n">
+        <v>25354</v>
+      </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="n">
@@ -22414,6 +23170,9 @@
       <c r="AA253" s="2" t="n">
         <v>15634</v>
       </c>
+      <c r="AB253" s="2" t="n">
+        <v>15752</v>
+      </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="n">
@@ -22497,6 +23256,9 @@
       <c r="AA254" s="2" t="n">
         <v>16121</v>
       </c>
+      <c r="AB254" s="2" t="n">
+        <v>16277</v>
+      </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="n">
@@ -22580,6 +23342,9 @@
       <c r="AA255" s="2" t="n">
         <v>19068</v>
       </c>
+      <c r="AB255" s="2" t="n">
+        <v>19259</v>
+      </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="n">
@@ -22663,6 +23428,9 @@
       <c r="AA256" s="2" t="n">
         <v>9178</v>
       </c>
+      <c r="AB256" s="2" t="n">
+        <v>9289</v>
+      </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="n">
@@ -22746,6 +23514,9 @@
       <c r="AA257" s="2" t="n">
         <v>4493</v>
       </c>
+      <c r="AB257" s="2" t="n">
+        <v>4526</v>
+      </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="n">
@@ -22829,6 +23600,9 @@
       <c r="AA258" s="2" t="n">
         <v>14668</v>
       </c>
+      <c r="AB258" s="2" t="n">
+        <v>14860</v>
+      </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="n">
@@ -22912,6 +23686,9 @@
       <c r="AA259" s="2" t="n">
         <v>7098</v>
       </c>
+      <c r="AB259" s="2" t="n">
+        <v>7095</v>
+      </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="n">
@@ -22995,6 +23772,9 @@
       <c r="AA260" s="2" t="n">
         <v>5580</v>
       </c>
+      <c r="AB260" s="2" t="n">
+        <v>5601</v>
+      </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="n">
@@ -23078,6 +23858,9 @@
       <c r="AA261" s="2" t="n">
         <v>3660</v>
       </c>
+      <c r="AB261" s="2" t="n">
+        <v>3665</v>
+      </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="n">
@@ -23161,6 +23944,9 @@
       <c r="AA262" s="2" t="n">
         <v>27108</v>
       </c>
+      <c r="AB262" s="2" t="n">
+        <v>27039</v>
+      </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="n">
@@ -23244,6 +24030,9 @@
       <c r="AA263" s="2" t="n">
         <v>7957</v>
       </c>
+      <c r="AB263" s="2" t="n">
+        <v>7939</v>
+      </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="n">
@@ -23327,6 +24116,9 @@
       <c r="AA264" s="2" t="n">
         <v>622</v>
       </c>
+      <c r="AB264" s="2" t="n">
+        <v>621</v>
+      </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="n">
@@ -23410,6 +24202,9 @@
       <c r="AA265" s="2" t="n">
         <v>3788</v>
       </c>
+      <c r="AB265" s="2" t="n">
+        <v>3804</v>
+      </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="n">
@@ -23493,6 +24288,9 @@
       <c r="AA266" s="2" t="n">
         <v>5389</v>
       </c>
+      <c r="AB266" s="2" t="n">
+        <v>5402</v>
+      </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="n">
@@ -23576,6 +24374,9 @@
       <c r="AA267" s="2" t="n">
         <v>4632</v>
       </c>
+      <c r="AB267" s="2" t="n">
+        <v>4628</v>
+      </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="n">
@@ -23659,6 +24460,9 @@
       <c r="AA268" s="2" t="n">
         <v>2962</v>
       </c>
+      <c r="AB268" s="2" t="n">
+        <v>2950</v>
+      </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="n">
@@ -23742,6 +24546,9 @@
       <c r="AA269" s="2" t="n">
         <v>2519</v>
       </c>
+      <c r="AB269" s="2" t="n">
+        <v>2506</v>
+      </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="n">
@@ -23825,6 +24632,9 @@
       <c r="AA270" s="2" t="n">
         <v>5731</v>
       </c>
+      <c r="AB270" s="2" t="n">
+        <v>5747</v>
+      </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="n">
@@ -23908,6 +24718,9 @@
       <c r="AA271" s="2" t="n">
         <v>1962</v>
       </c>
+      <c r="AB271" s="2" t="n">
+        <v>1964</v>
+      </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="n">
@@ -23991,6 +24804,9 @@
       <c r="AA272" s="2" t="n">
         <v>6361</v>
       </c>
+      <c r="AB272" s="2" t="n">
+        <v>6362</v>
+      </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="n">
@@ -24074,6 +24890,9 @@
       <c r="AA273" s="2" t="n">
         <v>4575</v>
       </c>
+      <c r="AB273" s="2" t="n">
+        <v>4584</v>
+      </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="n">
@@ -24157,6 +24976,9 @@
       <c r="AA274" s="2" t="n">
         <v>5963</v>
       </c>
+      <c r="AB274" s="2" t="n">
+        <v>5989</v>
+      </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="n">
@@ -24240,6 +25062,9 @@
       <c r="AA275" s="2" t="n">
         <v>6865</v>
       </c>
+      <c r="AB275" s="2" t="n">
+        <v>6916</v>
+      </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="n">
@@ -24323,6 +25148,9 @@
       <c r="AA276" s="2" t="n">
         <v>2696</v>
       </c>
+      <c r="AB276" s="2" t="n">
+        <v>2710</v>
+      </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="n">
@@ -24406,6 +25234,9 @@
       <c r="AA277" s="2" t="n">
         <v>29184</v>
       </c>
+      <c r="AB277" s="2" t="n">
+        <v>29275</v>
+      </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="n">
@@ -24489,6 +25320,9 @@
       <c r="AA278" s="2" t="n">
         <v>11231</v>
       </c>
+      <c r="AB278" s="2" t="n">
+        <v>11360</v>
+      </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="n">
@@ -24572,6 +25406,9 @@
       <c r="AA279" s="2" t="n">
         <v>2680</v>
       </c>
+      <c r="AB279" s="2" t="n">
+        <v>2705</v>
+      </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="n">
@@ -24655,6 +25492,9 @@
       <c r="AA280" s="2" t="n">
         <v>4199</v>
       </c>
+      <c r="AB280" s="2" t="n">
+        <v>4234</v>
+      </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="n">
@@ -24738,6 +25578,9 @@
       <c r="AA281" s="2" t="n">
         <v>2998</v>
       </c>
+      <c r="AB281" s="2" t="n">
+        <v>3021</v>
+      </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="n">
@@ -24821,6 +25664,9 @@
       <c r="AA282" s="2" t="n">
         <v>26916</v>
       </c>
+      <c r="AB282" s="2" t="n">
+        <v>27037</v>
+      </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="n">
@@ -24904,6 +25750,9 @@
       <c r="AA283" s="2" t="n">
         <v>11528</v>
       </c>
+      <c r="AB283" s="2" t="n">
+        <v>11632</v>
+      </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="n">
@@ -24987,6 +25836,9 @@
       <c r="AA284" s="2" t="n">
         <v>7742</v>
       </c>
+      <c r="AB284" s="2" t="n">
+        <v>7834</v>
+      </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="n">
@@ -25070,6 +25922,9 @@
       <c r="AA285" s="2" t="n">
         <v>452</v>
       </c>
+      <c r="AB285" s="2" t="n">
+        <v>456</v>
+      </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="n">
@@ -25153,6 +26008,9 @@
       <c r="AA286" s="2" t="n">
         <v>19060</v>
       </c>
+      <c r="AB286" s="2" t="n">
+        <v>18988</v>
+      </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="n">
@@ -25236,6 +26094,9 @@
       <c r="AA287" s="2" t="n">
         <v>29996</v>
       </c>
+      <c r="AB287" s="2" t="n">
+        <v>30276</v>
+      </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="n">
@@ -25319,6 +26180,9 @@
       <c r="AA288" s="2" t="n">
         <v>59424</v>
       </c>
+      <c r="AB288" s="2" t="n">
+        <v>60166</v>
+      </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="n">
@@ -25402,6 +26266,9 @@
       <c r="AA289" s="2" t="n">
         <v>35208</v>
       </c>
+      <c r="AB289" s="2" t="n">
+        <v>35618</v>
+      </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="n">
@@ -25485,6 +26352,9 @@
       <c r="AA290" s="2" t="n">
         <v>958</v>
       </c>
+      <c r="AB290" s="2" t="n">
+        <v>972</v>
+      </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="n">
@@ -25568,6 +26438,9 @@
       <c r="AA291" s="2" t="n">
         <v>5088</v>
       </c>
+      <c r="AB291" s="2" t="n">
+        <v>5099</v>
+      </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="n">
@@ -25651,6 +26524,9 @@
       <c r="AA292" s="2" t="n">
         <v>11856</v>
       </c>
+      <c r="AB292" s="2" t="n">
+        <v>12026</v>
+      </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="n">
@@ -25734,6 +26610,9 @@
       <c r="AA293" s="2" t="n">
         <v>9965</v>
       </c>
+      <c r="AB293" s="2" t="n">
+        <v>10105</v>
+      </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="n">
@@ -25817,6 +26696,9 @@
       <c r="AA294" s="2" t="n">
         <v>5439</v>
       </c>
+      <c r="AB294" s="2" t="n">
+        <v>5507</v>
+      </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="n">
@@ -25900,6 +26782,9 @@
       <c r="AA295" s="2" t="n">
         <v>8427</v>
       </c>
+      <c r="AB295" s="2" t="n">
+        <v>8524</v>
+      </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="n">
@@ -25983,6 +26868,9 @@
       <c r="AA296" s="2" t="n">
         <v>6836</v>
       </c>
+      <c r="AB296" s="2" t="n">
+        <v>6929</v>
+      </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="n">
@@ -26066,6 +26954,9 @@
       <c r="AA297" s="2" t="n">
         <v>5070</v>
       </c>
+      <c r="AB297" s="2" t="n">
+        <v>5050</v>
+      </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="n">
@@ -26149,6 +27040,9 @@
       <c r="AA298" s="2" t="n">
         <v>8004</v>
       </c>
+      <c r="AB298" s="2" t="n">
+        <v>8072</v>
+      </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="n">
@@ -26232,6 +27126,9 @@
       <c r="AA299" s="2" t="n">
         <v>7919</v>
       </c>
+      <c r="AB299" s="2" t="n">
+        <v>7988</v>
+      </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="n">
@@ -26315,6 +27212,9 @@
       <c r="AA300" s="2" t="n">
         <v>2808</v>
       </c>
+      <c r="AB300" s="2" t="n">
+        <v>2832</v>
+      </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="n">
@@ -26398,6 +27298,9 @@
       <c r="AA301" s="2" t="n">
         <v>7889</v>
       </c>
+      <c r="AB301" s="2" t="n">
+        <v>7953</v>
+      </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="n">
@@ -26481,6 +27384,9 @@
       <c r="AA302" s="2" t="n">
         <v>9173</v>
       </c>
+      <c r="AB302" s="2" t="n">
+        <v>9264</v>
+      </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="n">
@@ -26564,6 +27470,9 @@
       <c r="AA303" s="2" t="n">
         <v>4432</v>
       </c>
+      <c r="AB303" s="2" t="n">
+        <v>4477</v>
+      </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="n">
@@ -26647,6 +27556,9 @@
       <c r="AA304" s="2" t="n">
         <v>4166</v>
       </c>
+      <c r="AB304" s="2" t="n">
+        <v>4199</v>
+      </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="n">
@@ -26730,6 +27642,9 @@
       <c r="AA305" s="2" t="n">
         <v>6371</v>
       </c>
+      <c r="AB305" s="2" t="n">
+        <v>6394</v>
+      </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="n">
@@ -26813,6 +27728,9 @@
       <c r="AA306" s="2" t="n">
         <v>6913</v>
       </c>
+      <c r="AB306" s="2" t="n">
+        <v>7016</v>
+      </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="n">
@@ -26896,6 +27814,9 @@
       <c r="AA307" s="2" t="n">
         <v>9191</v>
       </c>
+      <c r="AB307" s="2" t="n">
+        <v>9308</v>
+      </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="n">
@@ -26979,6 +27900,9 @@
       <c r="AA308" s="2" t="n">
         <v>11669</v>
       </c>
+      <c r="AB308" s="2" t="n">
+        <v>11842</v>
+      </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="n">
@@ -27062,6 +27986,9 @@
       <c r="AA309" s="2" t="n">
         <v>3647</v>
       </c>
+      <c r="AB309" s="2" t="n">
+        <v>3699</v>
+      </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="n">
@@ -27145,6 +28072,9 @@
       <c r="AA310" s="2" t="n">
         <v>5546</v>
       </c>
+      <c r="AB310" s="2" t="n">
+        <v>5619</v>
+      </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="n">
@@ -27228,6 +28158,9 @@
       <c r="AA311" s="2" t="n">
         <v>10748</v>
       </c>
+      <c r="AB311" s="2" t="n">
+        <v>10787</v>
+      </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="n">
@@ -27311,6 +28244,9 @@
       <c r="AA312" s="2" t="n">
         <v>14151</v>
       </c>
+      <c r="AB312" s="2" t="n">
+        <v>14331</v>
+      </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="n">
@@ -27394,6 +28330,9 @@
       <c r="AA313" s="2" t="n">
         <v>10394</v>
       </c>
+      <c r="AB313" s="2" t="n">
+        <v>10534</v>
+      </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="n">
@@ -27477,6 +28416,9 @@
       <c r="AA314" s="2" t="n">
         <v>12848</v>
       </c>
+      <c r="AB314" s="2" t="n">
+        <v>13017</v>
+      </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="n">
@@ -27560,6 +28502,9 @@
       <c r="AA315" s="2" t="n">
         <v>7782</v>
       </c>
+      <c r="AB315" s="2" t="n">
+        <v>7891</v>
+      </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="n">
@@ -27643,6 +28588,9 @@
       <c r="AA316" s="2" t="n">
         <v>6399</v>
       </c>
+      <c r="AB316" s="2" t="n">
+        <v>6413</v>
+      </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="n">
@@ -27726,6 +28674,9 @@
       <c r="AA317" s="2" t="n">
         <v>8794</v>
       </c>
+      <c r="AB317" s="2" t="n">
+        <v>8895</v>
+      </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="n">
@@ -27809,6 +28760,9 @@
       <c r="AA318" s="2" t="n">
         <v>3083</v>
       </c>
+      <c r="AB318" s="2" t="n">
+        <v>3115</v>
+      </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="n">
@@ -27892,6 +28846,9 @@
       <c r="AA319" s="2" t="n">
         <v>5172</v>
       </c>
+      <c r="AB319" s="2" t="n">
+        <v>5232</v>
+      </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="n">
@@ -27975,6 +28932,9 @@
       <c r="AA320" s="2" t="n">
         <v>11583</v>
       </c>
+      <c r="AB320" s="2" t="n">
+        <v>11625</v>
+      </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="n">
@@ -28058,6 +29018,9 @@
       <c r="AA321" s="2" t="n">
         <v>7669</v>
       </c>
+      <c r="AB321" s="2" t="n">
+        <v>7753</v>
+      </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="n">
@@ -28141,6 +29104,9 @@
       <c r="AA322" s="2" t="n">
         <v>7410</v>
       </c>
+      <c r="AB322" s="2" t="n">
+        <v>7475</v>
+      </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="n">
@@ -28224,6 +29190,9 @@
       <c r="AA323" s="2" t="n">
         <v>8318</v>
       </c>
+      <c r="AB323" s="2" t="n">
+        <v>8341</v>
+      </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="n">
@@ -28307,6 +29276,9 @@
       <c r="AA324" s="2" t="n">
         <v>5281</v>
       </c>
+      <c r="AB324" s="2" t="n">
+        <v>5340</v>
+      </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="n">
@@ -28390,6 +29362,9 @@
       <c r="AA325" s="2" t="n">
         <v>11548</v>
       </c>
+      <c r="AB325" s="2" t="n">
+        <v>11720</v>
+      </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="0" t="n">
@@ -28473,6 +29448,9 @@
       <c r="AA326" s="2" t="n">
         <v>21427</v>
       </c>
+      <c r="AB326" s="2" t="n">
+        <v>21485</v>
+      </c>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="0" t="n">
@@ -28556,6 +29534,9 @@
       <c r="AA327" s="2" t="n">
         <v>9941</v>
       </c>
+      <c r="AB327" s="2" t="n">
+        <v>10034</v>
+      </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="n">
@@ -28639,6 +29620,9 @@
       <c r="AA328" s="2" t="n">
         <v>30682</v>
       </c>
+      <c r="AB328" s="2" t="n">
+        <v>31580</v>
+      </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="n">
@@ -28722,6 +29706,9 @@
       <c r="AA329" s="2" t="n">
         <v>16074</v>
       </c>
+      <c r="AB329" s="2" t="n">
+        <v>16493</v>
+      </c>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="n">
@@ -28805,6 +29792,9 @@
       <c r="AA330" s="2" t="n">
         <v>35036</v>
       </c>
+      <c r="AB330" s="2" t="n">
+        <v>35957</v>
+      </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="n">
@@ -28888,6 +29878,9 @@
       <c r="AA331" s="2" t="n">
         <v>2006</v>
       </c>
+      <c r="AB331" s="2" t="n">
+        <v>2059</v>
+      </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="0" t="n">
@@ -28971,6 +29964,9 @@
       <c r="AA332" s="2" t="n">
         <v>1553</v>
       </c>
+      <c r="AB332" s="2" t="n">
+        <v>1598</v>
+      </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="n">
@@ -29054,6 +30050,9 @@
       <c r="AA333" s="2" t="n">
         <v>66040</v>
       </c>
+      <c r="AB333" s="2" t="n">
+        <v>67132</v>
+      </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="n">
@@ -29137,6 +30136,9 @@
       <c r="AA334" s="2" t="n">
         <v>4017</v>
       </c>
+      <c r="AB334" s="2" t="n">
+        <v>4075</v>
+      </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="n">
@@ -29220,6 +30222,9 @@
       <c r="AA335" s="2" t="n">
         <v>2002</v>
       </c>
+      <c r="AB335" s="2" t="n">
+        <v>2032</v>
+      </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="n">
@@ -29303,6 +30308,9 @@
       <c r="AA336" s="2" t="n">
         <v>3062</v>
       </c>
+      <c r="AB336" s="2" t="n">
+        <v>3129</v>
+      </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="0" t="n">
@@ -29386,6 +30394,9 @@
       <c r="AA337" s="2" t="n">
         <v>3191</v>
       </c>
+      <c r="AB337" s="2" t="n">
+        <v>3242</v>
+      </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="n">
@@ -29469,6 +30480,9 @@
       <c r="AA338" s="2" t="n">
         <v>26919</v>
       </c>
+      <c r="AB338" s="2" t="n">
+        <v>27131</v>
+      </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="0" t="n">
@@ -29552,6 +30566,9 @@
       <c r="AA339" s="2" t="n">
         <v>5774</v>
       </c>
+      <c r="AB339" s="2" t="n">
+        <v>5772</v>
+      </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="0" t="n">
@@ -29635,6 +30652,9 @@
       <c r="AA340" s="2" t="n">
         <v>7123</v>
       </c>
+      <c r="AB340" s="2" t="n">
+        <v>7148</v>
+      </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="0" t="n">
@@ -29718,6 +30738,9 @@
       <c r="AA341" s="2" t="n">
         <v>2587</v>
       </c>
+      <c r="AB341" s="2" t="n">
+        <v>2591</v>
+      </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="0" t="n">
@@ -29801,6 +30824,9 @@
       <c r="AA342" s="2" t="n">
         <v>4627</v>
       </c>
+      <c r="AB342" s="2" t="n">
+        <v>4685</v>
+      </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="0" t="n">
@@ -29884,6 +30910,9 @@
       <c r="AA343" s="2" t="n">
         <v>7044</v>
       </c>
+      <c r="AB343" s="2" t="n">
+        <v>7213</v>
+      </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="0" t="n">
@@ -29967,6 +30996,9 @@
       <c r="AA344" s="2" t="n">
         <v>3051</v>
       </c>
+      <c r="AB344" s="2" t="n">
+        <v>3084</v>
+      </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="0" t="n">
@@ -30050,6 +31082,9 @@
       <c r="AA345" s="2" t="n">
         <v>27645</v>
       </c>
+      <c r="AB345" s="2" t="n">
+        <v>28008</v>
+      </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="0" t="n">
@@ -30133,6 +31168,9 @@
       <c r="AA346" s="2" t="n">
         <v>2149</v>
       </c>
+      <c r="AB346" s="2" t="n">
+        <v>2182</v>
+      </c>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="0" t="n">
@@ -30216,6 +31254,9 @@
       <c r="AA347" s="2" t="n">
         <v>9108</v>
       </c>
+      <c r="AB347" s="2" t="n">
+        <v>9302</v>
+      </c>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="0" t="n">
@@ -30299,6 +31340,9 @@
       <c r="AA348" s="2" t="n">
         <v>6354</v>
       </c>
+      <c r="AB348" s="2" t="n">
+        <v>6467</v>
+      </c>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="0" t="n">
@@ -30382,6 +31426,9 @@
       <c r="AA349" s="2" t="n">
         <v>5039</v>
       </c>
+      <c r="AB349" s="2" t="n">
+        <v>5147</v>
+      </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="0" t="n">
@@ -30465,6 +31512,9 @@
       <c r="AA350" s="2" t="n">
         <v>2614</v>
       </c>
+      <c r="AB350" s="2" t="n">
+        <v>2678</v>
+      </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="0" t="n">
@@ -30548,6 +31598,9 @@
       <c r="AA351" s="2" t="n">
         <v>4910</v>
       </c>
+      <c r="AB351" s="2" t="n">
+        <v>4983</v>
+      </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="0" t="n">
@@ -30631,6 +31684,9 @@
       <c r="AA352" s="2" t="n">
         <v>4303</v>
       </c>
+      <c r="AB352" s="2" t="n">
+        <v>4381</v>
+      </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="0" t="n">
@@ -30714,6 +31770,9 @@
       <c r="AA353" s="2" t="n">
         <v>8003</v>
       </c>
+      <c r="AB353" s="2" t="n">
+        <v>8136</v>
+      </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="0" t="n">
@@ -30797,6 +31856,9 @@
       <c r="AA354" s="2" t="n">
         <v>16162</v>
       </c>
+      <c r="AB354" s="2" t="n">
+        <v>16462</v>
+      </c>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="0" t="n">
@@ -30880,6 +31942,9 @@
       <c r="AA355" s="2" t="n">
         <v>3093</v>
       </c>
+      <c r="AB355" s="2" t="n">
+        <v>3112</v>
+      </c>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="0" t="n">
@@ -30963,6 +32028,9 @@
       <c r="AA356" s="2" t="n">
         <v>4052</v>
       </c>
+      <c r="AB356" s="2" t="n">
+        <v>4079</v>
+      </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="0" t="n">
@@ -31046,6 +32114,9 @@
       <c r="AA357" s="2" t="n">
         <v>1187</v>
       </c>
+      <c r="AB357" s="2" t="n">
+        <v>1194</v>
+      </c>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="0" t="n">
@@ -31129,6 +32200,9 @@
       <c r="AA358" s="2" t="n">
         <v>8889</v>
       </c>
+      <c r="AB358" s="2" t="n">
+        <v>8967</v>
+      </c>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="0" t="n">
@@ -31212,6 +32286,9 @@
       <c r="AA359" s="2" t="n">
         <v>6753</v>
       </c>
+      <c r="AB359" s="2" t="n">
+        <v>6910</v>
+      </c>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="0" t="n">
@@ -31295,6 +32372,9 @@
       <c r="AA360" s="2" t="n">
         <v>19697</v>
       </c>
+      <c r="AB360" s="2" t="n">
+        <v>20094</v>
+      </c>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="0" t="n">
@@ -31378,6 +32458,9 @@
       <c r="AA361" s="2" t="n">
         <v>11516</v>
       </c>
+      <c r="AB361" s="2" t="n">
+        <v>11785</v>
+      </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="0" t="n">
@@ -31461,6 +32544,9 @@
       <c r="AA362" s="2" t="n">
         <v>26279</v>
       </c>
+      <c r="AB362" s="2" t="n">
+        <v>26577</v>
+      </c>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="0" t="n">
@@ -31544,6 +32630,9 @@
       <c r="AA363" s="2" t="n">
         <v>1349</v>
       </c>
+      <c r="AB363" s="2" t="n">
+        <v>1361</v>
+      </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0" t="n">
@@ -31627,6 +32716,9 @@
       <c r="AA364" s="2" t="n">
         <v>2059</v>
       </c>
+      <c r="AB364" s="2" t="n">
+        <v>2076</v>
+      </c>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="0" t="n">
@@ -31710,6 +32802,9 @@
       <c r="AA365" s="2" t="n">
         <v>2562</v>
       </c>
+      <c r="AB365" s="2" t="n">
+        <v>2582</v>
+      </c>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="0" t="n">
@@ -31793,6 +32888,9 @@
       <c r="AA366" s="2" t="n">
         <v>793</v>
       </c>
+      <c r="AB366" s="2" t="n">
+        <v>797</v>
+      </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="0" t="n">
@@ -31876,6 +32974,9 @@
       <c r="AA367" s="2" t="n">
         <v>10379</v>
       </c>
+      <c r="AB367" s="2" t="n">
+        <v>10437</v>
+      </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="0" t="n">
@@ -31959,6 +33060,9 @@
       <c r="AA368" s="2" t="n">
         <v>2805</v>
       </c>
+      <c r="AB368" s="2" t="n">
+        <v>2827</v>
+      </c>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="0" t="n">
@@ -32042,6 +33146,9 @@
       <c r="AA369" s="2" t="n">
         <v>1842</v>
       </c>
+      <c r="AB369" s="2" t="n">
+        <v>1857</v>
+      </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="0" t="n">
@@ -32125,6 +33232,9 @@
       <c r="AA370" s="2" t="n">
         <v>5128</v>
       </c>
+      <c r="AB370" s="2" t="n">
+        <v>5161</v>
+      </c>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="0" t="n">
@@ -32208,6 +33318,9 @@
       <c r="AA371" s="2" t="n">
         <v>9394</v>
       </c>
+      <c r="AB371" s="2" t="n">
+        <v>9449</v>
+      </c>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="0" t="n">
@@ -32291,6 +33404,9 @@
       <c r="AA372" s="2" t="n">
         <v>3085</v>
       </c>
+      <c r="AB372" s="2" t="n">
+        <v>3104</v>
+      </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="0" t="n">
@@ -32374,6 +33490,9 @@
       <c r="AA373" s="2" t="n">
         <v>2017</v>
       </c>
+      <c r="AB373" s="2" t="n">
+        <v>2029</v>
+      </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="0" t="n">
@@ -32457,6 +33576,9 @@
       <c r="AA374" s="2" t="n">
         <v>2174</v>
       </c>
+      <c r="AB374" s="2" t="n">
+        <v>2188</v>
+      </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="0" t="n">
@@ -32540,6 +33662,9 @@
       <c r="AA375" s="2" t="n">
         <v>959</v>
       </c>
+      <c r="AB375" s="2" t="n">
+        <v>958</v>
+      </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="0" t="n">
@@ -32623,6 +33748,9 @@
       <c r="AA376" s="2" t="n">
         <v>1538</v>
       </c>
+      <c r="AB376" s="2" t="n">
+        <v>1545</v>
+      </c>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="0" t="n">
@@ -32706,6 +33834,9 @@
       <c r="AA377" s="2" t="n">
         <v>2696</v>
       </c>
+      <c r="AB377" s="2" t="n">
+        <v>2711</v>
+      </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="0" t="n">
@@ -32789,6 +33920,9 @@
       <c r="AA378" s="2" t="n">
         <v>2642</v>
       </c>
+      <c r="AB378" s="2" t="n">
+        <v>2663</v>
+      </c>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="0" t="n">
@@ -32872,6 +34006,9 @@
       <c r="AA379" s="2" t="n">
         <v>1481</v>
       </c>
+      <c r="AB379" s="2" t="n">
+        <v>1480</v>
+      </c>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="0" t="n">
@@ -32955,6 +34092,9 @@
       <c r="AA380" s="2" t="n">
         <v>1261</v>
       </c>
+      <c r="AB380" s="2" t="n">
+        <v>1263</v>
+      </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="0" t="n">
@@ -33038,6 +34178,9 @@
       <c r="AA381" s="2" t="n">
         <v>2356</v>
       </c>
+      <c r="AB381" s="2" t="n">
+        <v>2362</v>
+      </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="0" t="n">
@@ -33121,6 +34264,9 @@
       <c r="AA382" s="2" t="n">
         <v>761</v>
       </c>
+      <c r="AB382" s="2" t="n">
+        <v>759</v>
+      </c>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="0" t="n">
@@ -33204,6 +34350,9 @@
       <c r="AA383" s="2" t="n">
         <v>3314</v>
       </c>
+      <c r="AB383" s="2" t="n">
+        <v>3311</v>
+      </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="0" t="n">
@@ -33287,6 +34436,9 @@
       <c r="AA384" s="2" t="n">
         <v>12968</v>
       </c>
+      <c r="AB384" s="2" t="n">
+        <v>13204</v>
+      </c>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="0" t="n">
@@ -33370,6 +34522,9 @@
       <c r="AA385" s="2" t="n">
         <v>9038</v>
       </c>
+      <c r="AB385" s="2" t="n">
+        <v>9191</v>
+      </c>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="0" t="n">
@@ -33453,6 +34608,9 @@
       <c r="AA386" s="2" t="n">
         <v>2614</v>
       </c>
+      <c r="AB386" s="2" t="n">
+        <v>2665</v>
+      </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="0" t="n">
@@ -33536,6 +34694,9 @@
       <c r="AA387" s="2" t="n">
         <v>2961</v>
       </c>
+      <c r="AB387" s="2" t="n">
+        <v>3011</v>
+      </c>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="0" t="n">
@@ -33619,6 +34780,9 @@
       <c r="AA388" s="2" t="n">
         <v>4673</v>
       </c>
+      <c r="AB388" s="2" t="n">
+        <v>4707</v>
+      </c>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="0" t="n">
@@ -33702,6 +34866,9 @@
       <c r="AA389" s="2" t="n">
         <v>728</v>
       </c>
+      <c r="AB389" s="2" t="n">
+        <v>724</v>
+      </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="0" t="n">
@@ -33785,6 +34952,9 @@
       <c r="AA390" s="2" t="n">
         <v>1883</v>
       </c>
+      <c r="AB390" s="2" t="n">
+        <v>1893</v>
+      </c>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="0" t="n">
@@ -33868,6 +35038,9 @@
       <c r="AA391" s="2" t="n">
         <v>759</v>
       </c>
+      <c r="AB391" s="2" t="n">
+        <v>761</v>
+      </c>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="0" t="n">
@@ -33951,6 +35124,9 @@
       <c r="AA392" s="2" t="n">
         <v>10288</v>
       </c>
+      <c r="AB392" s="2" t="n">
+        <v>10342</v>
+      </c>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="n">
@@ -34034,6 +35210,9 @@
       <c r="AA393" s="2" t="n">
         <v>2712</v>
       </c>
+      <c r="AB393" s="2" t="n">
+        <v>2755</v>
+      </c>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="n">
@@ -34117,6 +35296,9 @@
       <c r="AA394" s="2" t="n">
         <v>6573</v>
       </c>
+      <c r="AB394" s="2" t="n">
+        <v>6645</v>
+      </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="n">
@@ -34200,6 +35382,9 @@
       <c r="AA395" s="2" t="n">
         <v>10396</v>
       </c>
+      <c r="AB395" s="2" t="n">
+        <v>10444</v>
+      </c>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="0" t="n">
@@ -34283,6 +35468,9 @@
       <c r="AA396" s="2" t="n">
         <v>8318</v>
       </c>
+      <c r="AB396" s="2" t="n">
+        <v>8410</v>
+      </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="n">
@@ -34366,6 +35554,9 @@
       <c r="AA397" s="2" t="n">
         <v>3418</v>
       </c>
+      <c r="AB397" s="2" t="n">
+        <v>3459</v>
+      </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="n">
@@ -34449,6 +35640,9 @@
       <c r="AA398" s="2" t="n">
         <v>1166</v>
       </c>
+      <c r="AB398" s="2" t="n">
+        <v>1173</v>
+      </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="0" t="n">
@@ -34532,6 +35726,9 @@
       <c r="AA399" s="2" t="n">
         <v>38750</v>
       </c>
+      <c r="AB399" s="2" t="n">
+        <v>39426</v>
+      </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="0" t="n">
@@ -34615,6 +35812,9 @@
       <c r="AA400" s="2" t="n">
         <v>4900</v>
       </c>
+      <c r="AB400" s="2" t="n">
+        <v>4943</v>
+      </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="n">
@@ -34698,6 +35898,9 @@
       <c r="AA401" s="2" t="n">
         <v>9626</v>
       </c>
+      <c r="AB401" s="2" t="n">
+        <v>9736</v>
+      </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="n">
@@ -34781,6 +35984,9 @@
       <c r="AA402" s="2" t="n">
         <v>20918</v>
       </c>
+      <c r="AB402" s="2" t="n">
+        <v>21244</v>
+      </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="0" t="n">
@@ -34864,6 +36070,9 @@
       <c r="AA403" s="2" t="n">
         <v>1704</v>
       </c>
+      <c r="AB403" s="2" t="n">
+        <v>1714</v>
+      </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="n">
@@ -34947,6 +36156,9 @@
       <c r="AA404" s="2" t="n">
         <v>1546</v>
       </c>
+      <c r="AB404" s="2" t="n">
+        <v>1560</v>
+      </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="0" t="n">
@@ -35030,6 +36242,9 @@
       <c r="AA405" s="2" t="n">
         <v>20920</v>
       </c>
+      <c r="AB405" s="2" t="n">
+        <v>21240</v>
+      </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="0" t="n">
@@ -35113,6 +36328,9 @@
       <c r="AA406" s="2" t="n">
         <v>775</v>
       </c>
+      <c r="AB406" s="2" t="n">
+        <v>784</v>
+      </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="0" t="n">
@@ -35196,6 +36414,9 @@
       <c r="AA407" s="2" t="n">
         <v>21932</v>
       </c>
+      <c r="AB407" s="2" t="n">
+        <v>22181</v>
+      </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="n">
@@ -35279,6 +36500,9 @@
       <c r="AA408" s="2" t="n">
         <v>8761</v>
       </c>
+      <c r="AB408" s="2" t="n">
+        <v>8915</v>
+      </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="n">
@@ -35362,6 +36586,9 @@
       <c r="AA409" s="2" t="n">
         <v>5392</v>
       </c>
+      <c r="AB409" s="2" t="n">
+        <v>5482</v>
+      </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="n">
@@ -35445,6 +36672,9 @@
       <c r="AA410" s="2" t="n">
         <v>1701</v>
       </c>
+      <c r="AB410" s="2" t="n">
+        <v>1725</v>
+      </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="0" t="n">
@@ -35528,6 +36758,9 @@
       <c r="AA411" s="2" t="n">
         <v>928</v>
       </c>
+      <c r="AB411" s="2" t="n">
+        <v>941</v>
+      </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0" t="n">
@@ -35611,6 +36844,9 @@
       <c r="AA412" s="2" t="n">
         <v>28726</v>
       </c>
+      <c r="AB412" s="2" t="n">
+        <v>29454</v>
+      </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="n">
@@ -35694,6 +36930,9 @@
       <c r="AA413" s="2" t="n">
         <v>3715</v>
       </c>
+      <c r="AB413" s="2" t="n">
+        <v>3690</v>
+      </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="n">
@@ -35777,6 +37016,9 @@
       <c r="AA414" s="2" t="n">
         <v>6491</v>
       </c>
+      <c r="AB414" s="2" t="n">
+        <v>6494</v>
+      </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="0" t="n">
@@ -35860,6 +37102,9 @@
       <c r="AA415" s="2" t="n">
         <v>3287</v>
       </c>
+      <c r="AB415" s="2" t="n">
+        <v>3289</v>
+      </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="0" t="n">
@@ -35943,6 +37188,9 @@
       <c r="AA416" s="2" t="n">
         <v>1756</v>
       </c>
+      <c r="AB416" s="2" t="n">
+        <v>1749</v>
+      </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="n">
@@ -36026,6 +37274,9 @@
       <c r="AA417" s="2" t="n">
         <v>1396</v>
       </c>
+      <c r="AB417" s="2" t="n">
+        <v>1391</v>
+      </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="0" t="n">
@@ -36109,6 +37360,9 @@
       <c r="AA418" s="2" t="n">
         <v>2919</v>
       </c>
+      <c r="AB418" s="2" t="n">
+        <v>2929</v>
+      </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="0" t="n">
@@ -36192,6 +37446,9 @@
       <c r="AA419" s="2" t="n">
         <v>2599</v>
       </c>
+      <c r="AB419" s="2" t="n">
+        <v>2589</v>
+      </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="0" t="n">
@@ -36275,6 +37532,9 @@
       <c r="AA420" s="2" t="n">
         <v>3222</v>
       </c>
+      <c r="AB420" s="2" t="n">
+        <v>3197</v>
+      </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="0" t="n">
@@ -36358,6 +37618,9 @@
       <c r="AA421" s="2" t="n">
         <v>8962</v>
       </c>
+      <c r="AB421" s="2" t="n">
+        <v>9027</v>
+      </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="0" t="n">
@@ -36441,6 +37704,9 @@
       <c r="AA422" s="2" t="n">
         <v>1500</v>
       </c>
+      <c r="AB422" s="2" t="n">
+        <v>1513</v>
+      </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="0" t="n">
@@ -36524,6 +37790,9 @@
       <c r="AA423" s="2" t="n">
         <v>3994</v>
       </c>
+      <c r="AB423" s="2" t="n">
+        <v>4047</v>
+      </c>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="0" t="n">
@@ -36607,6 +37876,9 @@
       <c r="AA424" s="2" t="n">
         <v>8785</v>
       </c>
+      <c r="AB424" s="2" t="n">
+        <v>8844</v>
+      </c>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="0" t="n">
@@ -36690,6 +37962,9 @@
       <c r="AA425" s="2" t="n">
         <v>9719</v>
       </c>
+      <c r="AB425" s="2" t="n">
+        <v>9716</v>
+      </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="n">
@@ -36773,6 +38048,9 @@
       <c r="AA426" s="2" t="n">
         <v>3628</v>
       </c>
+      <c r="AB426" s="2" t="n">
+        <v>3645</v>
+      </c>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="n">
@@ -36856,6 +38134,9 @@
       <c r="AA427" s="2" t="n">
         <v>3468</v>
       </c>
+      <c r="AB427" s="2" t="n">
+        <v>3487</v>
+      </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="n">
@@ -36939,6 +38220,9 @@
       <c r="AA428" s="2" t="n">
         <v>4516</v>
       </c>
+      <c r="AB428" s="2" t="n">
+        <v>4529</v>
+      </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="n">
@@ -37022,6 +38306,9 @@
       <c r="AA429" s="2" t="n">
         <v>1154</v>
       </c>
+      <c r="AB429" s="2" t="n">
+        <v>1162</v>
+      </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="n">
@@ -37105,6 +38392,9 @@
       <c r="AA430" s="2" t="n">
         <v>25259</v>
       </c>
+      <c r="AB430" s="2" t="n">
+        <v>25665</v>
+      </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="0" t="n">
@@ -37188,6 +38478,9 @@
       <c r="AA431" s="2" t="n">
         <v>4077</v>
       </c>
+      <c r="AB431" s="2" t="n">
+        <v>4116</v>
+      </c>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="n">
@@ -37271,6 +38564,9 @@
       <c r="AA432" s="2" t="n">
         <v>4212</v>
       </c>
+      <c r="AB432" s="2" t="n">
+        <v>4239</v>
+      </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="0" t="n">
@@ -37354,6 +38650,9 @@
       <c r="AA433" s="2" t="n">
         <v>11861</v>
       </c>
+      <c r="AB433" s="2" t="n">
+        <v>11867</v>
+      </c>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0" t="n">
@@ -37437,6 +38736,9 @@
       <c r="AA434" s="2" t="n">
         <v>12519</v>
       </c>
+      <c r="AB434" s="2" t="n">
+        <v>12836</v>
+      </c>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="0" t="n">
@@ -37520,6 +38822,9 @@
       <c r="AA435" s="2" t="n">
         <v>14065</v>
       </c>
+      <c r="AB435" s="2" t="n">
+        <v>14120</v>
+      </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="0" t="n">
@@ -37603,6 +38908,9 @@
       <c r="AA436" s="2" t="n">
         <v>7602</v>
       </c>
+      <c r="AB436" s="2" t="n">
+        <v>7700</v>
+      </c>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="0" t="n">
@@ -37686,6 +38994,9 @@
       <c r="AA437" s="2" t="n">
         <v>16639</v>
       </c>
+      <c r="AB437" s="2" t="n">
+        <v>16629</v>
+      </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="0" t="n">
@@ -37769,6 +39080,9 @@
       <c r="AA438" s="2" t="n">
         <v>13194</v>
       </c>
+      <c r="AB438" s="2" t="n">
+        <v>13202</v>
+      </c>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="0" t="n">
@@ -37852,6 +39166,9 @@
       <c r="AA439" s="2" t="n">
         <v>7047</v>
       </c>
+      <c r="AB439" s="2" t="n">
+        <v>7050</v>
+      </c>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="n">
@@ -37935,6 +39252,9 @@
       <c r="AA440" s="2" t="n">
         <v>4149</v>
       </c>
+      <c r="AB440" s="2" t="n">
+        <v>4152</v>
+      </c>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="0" t="n">
@@ -38018,6 +39338,9 @@
       <c r="AA441" s="2" t="n">
         <v>3264</v>
       </c>
+      <c r="AB441" s="2" t="n">
+        <v>3247</v>
+      </c>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="0" t="n">
@@ -38101,6 +39424,9 @@
       <c r="AA442" s="2" t="n">
         <v>20594</v>
       </c>
+      <c r="AB442" s="2" t="n">
+        <v>20984</v>
+      </c>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="0" t="n">
@@ -38184,6 +39510,9 @@
       <c r="AA443" s="2" t="n">
         <v>19998</v>
       </c>
+      <c r="AB443" s="2" t="n">
+        <v>20050</v>
+      </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="0" t="n">
@@ -38267,6 +39596,9 @@
       <c r="AA444" s="2" t="n">
         <v>5254</v>
       </c>
+      <c r="AB444" s="2" t="n">
+        <v>5333</v>
+      </c>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="0" t="n">
@@ -38350,6 +39682,9 @@
       <c r="AA445" s="2" t="n">
         <v>15683</v>
       </c>
+      <c r="AB445" s="2" t="n">
+        <v>15929</v>
+      </c>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="0" t="n">
@@ -38433,6 +39768,9 @@
       <c r="AA446" s="2" t="n">
         <v>12017</v>
       </c>
+      <c r="AB446" s="2" t="n">
+        <v>12172</v>
+      </c>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="0" t="n">
@@ -38516,6 +39854,9 @@
       <c r="AA447" s="2" t="n">
         <v>26721</v>
       </c>
+      <c r="AB447" s="2" t="n">
+        <v>18613</v>
+      </c>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="0" t="n">
@@ -38599,6 +39940,9 @@
       <c r="AA448" s="2" t="n">
         <v>8577</v>
       </c>
+      <c r="AB448" s="2" t="n">
+        <v>8791</v>
+      </c>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="0" t="n">
@@ -38682,6 +40026,9 @@
       <c r="AA449" s="2" t="n">
         <v>60929</v>
       </c>
+      <c r="AB449" s="2" t="n">
+        <v>60710</v>
+      </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="0" t="n">
@@ -38765,6 +40112,9 @@
       <c r="AA450" s="2" t="n">
         <v>20617</v>
       </c>
+      <c r="AB450" s="2" t="n">
+        <v>20818</v>
+      </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="0" t="n">
@@ -38848,6 +40198,9 @@
       <c r="AA451" s="2" t="n">
         <v>10120</v>
       </c>
+      <c r="AB451" s="2" t="n">
+        <v>10257</v>
+      </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="0" t="n">
@@ -38931,6 +40284,9 @@
       <c r="AA452" s="2" t="n">
         <v>8375</v>
       </c>
+      <c r="AB452" s="2" t="n">
+        <v>8451</v>
+      </c>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="0" t="n">
@@ -39014,6 +40370,9 @@
       <c r="AA453" s="2" t="n">
         <v>38972</v>
       </c>
+      <c r="AB453" s="2" t="n">
+        <v>39611</v>
+      </c>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="0" t="n">
@@ -39097,6 +40456,9 @@
       <c r="AA454" s="2" t="n">
         <v>12887</v>
       </c>
+      <c r="AB454" s="2" t="n">
+        <v>13052</v>
+      </c>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="0" t="n">
@@ -39180,6 +40542,9 @@
       <c r="AA455" s="2" t="n">
         <v>28913</v>
       </c>
+      <c r="AB455" s="2" t="n">
+        <v>29241</v>
+      </c>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="0" t="n">
@@ -39263,6 +40628,9 @@
       <c r="AA456" s="2" t="n">
         <v>20115</v>
       </c>
+      <c r="AB456" s="2" t="n">
+        <v>20342</v>
+      </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="0" t="n">
@@ -39346,6 +40714,9 @@
       <c r="AA457" s="2" t="n">
         <v>39849</v>
       </c>
+      <c r="AB457" s="2" t="n">
+        <v>40278</v>
+      </c>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="0" t="n">
@@ -39429,6 +40800,9 @@
       <c r="AA458" s="2" t="n">
         <v>4980</v>
       </c>
+      <c r="AB458" s="2" t="n">
+        <v>5040</v>
+      </c>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="0" t="n">
@@ -39512,6 +40886,9 @@
       <c r="AA459" s="2" t="n">
         <v>6973</v>
       </c>
+      <c r="AB459" s="2" t="n">
+        <v>7110</v>
+      </c>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="0" t="n">
@@ -39595,6 +40972,9 @@
       <c r="AA460" s="2" t="n">
         <v>34523</v>
       </c>
+      <c r="AB460" s="2" t="n">
+        <v>34576</v>
+      </c>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="0" t="n">
@@ -39678,6 +41058,9 @@
       <c r="AA461" s="2" t="n">
         <v>10696</v>
       </c>
+      <c r="AB461" s="2" t="n">
+        <v>10804</v>
+      </c>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="0" t="n">
@@ -39761,6 +41144,9 @@
       <c r="AA462" s="2" t="n">
         <v>2635</v>
       </c>
+      <c r="AB462" s="2" t="n">
+        <v>2656</v>
+      </c>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="0" t="n">
@@ -39844,6 +41230,9 @@
       <c r="AA463" s="2" t="n">
         <v>3038</v>
       </c>
+      <c r="AB463" s="2" t="n">
+        <v>3062</v>
+      </c>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="0" t="n">
@@ -39927,6 +41316,9 @@
       <c r="AA464" s="2" t="n">
         <v>7540</v>
       </c>
+      <c r="AB464" s="2" t="n">
+        <v>7628</v>
+      </c>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="0" t="n">
@@ -40010,6 +41402,9 @@
       <c r="AA465" s="2" t="n">
         <v>6875</v>
       </c>
+      <c r="AB465" s="2" t="n">
+        <v>6947</v>
+      </c>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="0" t="n">
@@ -40093,6 +41488,9 @@
       <c r="AA466" s="2" t="n">
         <v>10356</v>
       </c>
+      <c r="AB466" s="2" t="n">
+        <v>10590</v>
+      </c>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="0" t="n">
@@ -40176,6 +41574,9 @@
       <c r="AA467" s="2" t="n">
         <v>11755</v>
       </c>
+      <c r="AB467" s="2" t="n">
+        <v>11847</v>
+      </c>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="0" t="n">
@@ -40259,6 +41660,9 @@
       <c r="AA468" s="2" t="n">
         <v>13341</v>
       </c>
+      <c r="AB468" s="2" t="n">
+        <v>13656</v>
+      </c>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="0" t="n">
@@ -40342,6 +41746,9 @@
       <c r="AA469" s="2" t="n">
         <v>8530</v>
       </c>
+      <c r="AB469" s="2" t="n">
+        <v>8709</v>
+      </c>
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="0" t="n">
@@ -40425,6 +41832,9 @@
       <c r="AA470" s="2" t="n">
         <v>10407</v>
       </c>
+      <c r="AB470" s="2" t="n">
+        <v>10437</v>
+      </c>
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="0" t="n">
@@ -40508,6 +41918,9 @@
       <c r="AA471" s="2" t="n">
         <v>20570</v>
       </c>
+      <c r="AB471" s="2" t="n">
+        <v>20814</v>
+      </c>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="0" t="n">
@@ -40591,6 +42004,9 @@
       <c r="AA472" s="2" t="n">
         <v>15913</v>
       </c>
+      <c r="AB472" s="2" t="n">
+        <v>16140</v>
+      </c>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="0" t="n">
@@ -40674,6 +42090,9 @@
       <c r="AA473" s="2" t="n">
         <v>25640</v>
       </c>
+      <c r="AB473" s="2" t="n">
+        <v>26152</v>
+      </c>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="0" t="n">
@@ -40757,6 +42176,9 @@
       <c r="AA474" s="2" t="n">
         <v>2334</v>
       </c>
+      <c r="AB474" s="2" t="n">
+        <v>2357</v>
+      </c>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="0" t="n">
@@ -40840,6 +42262,9 @@
       <c r="AA475" s="2" t="n">
         <v>8380</v>
       </c>
+      <c r="AB475" s="2" t="n">
+        <v>8494</v>
+      </c>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="0" t="n">
@@ -40923,6 +42348,9 @@
       <c r="AA476" s="2" t="n">
         <v>11665</v>
       </c>
+      <c r="AB476" s="2" t="n">
+        <v>11836</v>
+      </c>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="0" t="n">
@@ -41006,11 +42434,14 @@
       <c r="AA477" s="2" t="n">
         <v>8063</v>
       </c>
+      <c r="AB477" s="2" t="n">
+        <v>8182</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>